<commit_message>
ajuste nas labels do form
</commit_message>
<xml_diff>
--- a/reports/cliente_x_dia.xlsx
+++ b/reports/cliente_x_dia.xlsx
@@ -67,17 +67,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="20.68988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.789887640449443"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.38988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -115,245 +115,152 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>210.983.091-28</t>
-        </is>
+      <c r="A3" s="0" t="n">
+        <v>980</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>testerr</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>gabemil@gmail.com</t>
+          <t>r@r.com.br</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>(12) 3123-1231</t>
+          <t>(11) 1111-11111</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>(11) 2312-3123</t>
+          <t>(11) 1111-1111</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>210.983.091-28</t>
-        </is>
+      <c r="A4" s="0" t="n">
+        <v>131</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Rodrigo</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>gabemil@gmail.com</t>
+          <t>ro@ras.com</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>(12) 3123-1231</t>
+          <t>(21) 3123-12312</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>(11) 2312-3123</t>
+          <t>(12) 3123-1321</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>210.983.091-28</t>
-        </is>
+      <c r="A5" s="0" t="n">
+        <v>109</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>çlçlaskdçlk</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>gabemil@gmail.com</t>
+          <t>90831@12321.com</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>(12) 3123-1231</t>
+          <t/>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>(11) 2312-3123</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>019.820.182-09</t>
-        </is>
+      <c r="A6" s="0" t="n">
+        <v>311</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>Rodrigo Bruno de Souza</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>2@wqe.com</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>(11) 98293-1293</t>
+          <t>(12) 3123-123</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>(11) 12932-1290</t>
+          <t>(31) 2312-3131</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>491.029.809-12</t>
-        </is>
+      <c r="A7" s="0" t="n">
+        <v>123</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>kjkljlkj</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>dfs@xn--sdad-zoac.com</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>(11) 9012-1983</t>
+          <t>(11) 1111-11111</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>(11) 2941-1299</t>
+          <t>(12) 3111-1111</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="inlineStr">
-        <is>
-          <t>124.124.124-12</t>
-        </is>
+      <c r="A8" s="0" t="n">
+        <v>312</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>Rodrigo Bruno de Souza</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>r@r.com</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>(91) 8291-82912</t>
+          <t>(11) 1111-11111</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>(91) 2891-2821</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="inlineStr">
-        <is>
-          <t>190.283.019-28</t>
-        </is>
-      </c>
-      <c r="B9" s="0" t="inlineStr">
-        <is>
-          <t>Marcos</t>
-        </is>
-      </c>
-      <c r="C9" s="0" t="inlineStr">
-        <is>
-          <t>marcosdasilva@gmail.com</t>
-        </is>
-      </c>
-      <c r="D9" s="0" t="inlineStr">
-        <is>
-          <t>(91) 8291-82912</t>
-        </is>
-      </c>
-      <c r="E9" s="0" t="inlineStr">
-        <is>
-          <t>(91) 2891-2821</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="inlineStr">
-        <is>
-          <t>402.298.198-91</t>
-        </is>
-      </c>
-      <c r="B10" s="0" t="inlineStr">
-        <is>
-          <t>Thiago Santos Oliveira</t>
-        </is>
-      </c>
-      <c r="C10" s="0" t="inlineStr">
-        <is>
-          <t>thisantos@gmail.com</t>
-        </is>
-      </c>
-      <c r="D10" s="0" t="inlineStr">
-        <is>
-          <t>(11)9823-98233</t>
-        </is>
-      </c>
-      <c r="E10" s="0" t="inlineStr">
-        <is>
-          <t>(11)9823-98233</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="inlineStr">
-        <is>
-          <t>481.902.830-91</t>
-        </is>
-      </c>
-      <c r="B11" s="0" t="inlineStr">
-        <is>
-          <t>Thiago Santos Oliveira</t>
-        </is>
-      </c>
-      <c r="C11" s="0" t="inlineStr">
-        <is>
-          <t>thisantos@gmail.com</t>
-        </is>
-      </c>
-      <c r="D11" s="0" t="inlineStr">
-        <is>
-          <t>(01) 9283-09182</t>
-        </is>
-      </c>
-      <c r="E11" s="0" t="inlineStr">
-        <is>
-          <t>(10) 9283-0912</t>
+          <t>(23) 1111-1111</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
layout de cadastro de user ajustado e mais erros js resolvidos
</commit_message>
<xml_diff>
--- a/reports/cliente_x_dia.xlsx
+++ b/reports/cliente_x_dia.xlsx
@@ -67,17 +67,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="20.68988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.789887640449443"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.08988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.28988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -117,270 +117,397 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>123.871.983-27</t>
+          <t>313.213.213-2</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>sdasda</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>thiago@souza.com</t>
+          <t>123@sdasd</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>(29) 0182-90180</t>
+          <t>(13) 2132-1</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>(19) 8209-8109</t>
+          <t>(32) 1321-3213</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>210.983.091-28</t>
-        </is>
+      <c r="A4" s="0" t="n">
+        <v>321.3</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Rodrigo Bruno de Souza</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>gabemil@gmail.com</t>
+          <t>1@sdf.coms</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>(12) 3123-1231</t>
+          <t>(12) 3132-13213</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>(11) 2312-3123</t>
+          <t>(31) 321</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>210.983.091-28</t>
+          <t>321.321.321-32</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Rodrigo Bruno de Souza</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>gabemil@gmail.com</t>
+          <t>1321321@31321.com</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>(12) 3123-1231</t>
+          <t>(31) 3213-21321</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>(11) 2312-3123</t>
+          <t>(31) 3333-3333</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>210.983.091-28</t>
-        </is>
+      <c r="A6" s="0" t="n">
+        <v>3132</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>gabemil@gmail.com</t>
+          <t>r@r.com</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>(12) 3123-1231</t>
+          <t>(32) 1321-32132</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>(11) 2312-3123</t>
+          <t>(32) 1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>019.820.182-09</t>
+          <t>321.321.321</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>sdfsdf</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>1321321@asd</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>(11) 98293-1293</t>
+          <t>(32) 1321-23132</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>(11) 12932-1290</t>
+          <t>(32) 132</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>491.029.809-12</t>
+          <t>399.065.215-84</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>Rodrigo Bruno de Souza</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>ro_web1@fsa.com</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>(11) 9012-1983</t>
+          <t>(12) 1321-32132</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>(11) 2941-1299</t>
+          <t>(11) 9806-5588</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="inlineStr">
-        <is>
-          <t>124.124.124-12</t>
-        </is>
+      <c r="A9" s="0" t="n">
+        <v>33333333333333</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>a@sd.com</t>
         </is>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>(91) 8291-82912</t>
+          <t>(32) 1321-32132</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>(91) 2891-2821</t>
+          <t>(32) 1321</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>190.283.019-28</t>
+          <t>313.212.313-2</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>23a1d32asd1</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>marcosdasilva@gmail.com</t>
+          <t>asd@asdas.com</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>(91) 8291-82912</t>
+          <t>(32) 1321-321</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>(91) 2891-2821</t>
+          <t>(32) 1321-3213</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>402.298.198-91</t>
+          <t>321.321.321-31</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Thiago Santos Oliveira</t>
+          <t>32as1d3s2a1</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>thisantos@gmail.com</t>
+          <t>321321321321313@adsadas.com</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>(11)9823-98233</t>
+          <t>(32) 1321</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>(11)9823-98233</t>
+          <t>(31) 3213-21</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>481.902.830-91</t>
+          <t>313.213.213-21</t>
         </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Thiago Santos Oliveira</t>
+          <t>a23ds1s3a21</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>thisantos@gmail.com</t>
+          <t>313131@asddasd.com</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>(01) 9283-09182</t>
+          <t>(32) 1</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>(10) 9283-0912</t>
+          <t>(13) 21321</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>313.213.213</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>21321321</v>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>teste@dasdasd.com</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>(32) 1</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>(32) 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>333.333.333-33</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>asdsad</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>asdsa@adsad.com</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>(32) 1</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>(65) 321</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>313.213.21</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>sssdfsd</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>teste@sdsf.com</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>(31) 3213-2113</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>(32) 1321</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>3213132@sadasd</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>333.333.333</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>3213132@sadasd</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>(31) 3213-2</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>(32) 1321-321</t>
         </is>
       </c>
     </row>

</xml_diff>